<commit_message>
Nesta versão conseguimos cadastrar o nome da empresa e a data da realização dos exames dentro da planilha em excel
</commit_message>
<xml_diff>
--- a/excel_docs/teste.xlsx
+++ b/excel_docs/teste.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>PROTOCOLO DE EMPRESAS</t>
   </si>
@@ -29,6 +29,12 @@
     <t>DATA</t>
   </si>
   <si>
+    <t>asasa</t>
+  </si>
+  <si>
+    <t>0023-03-12</t>
+  </si>
+  <si>
     <t>NOME DO COLABORADOR</t>
   </si>
   <si>
@@ -38,22 +44,13 @@
     <t>ENTREGUE</t>
   </si>
   <si>
-    <t>Eduardo</t>
-  </si>
-  <si>
-    <t>ASO PER</t>
-  </si>
-  <si>
-    <t>Fernanda</t>
-  </si>
-  <si>
-    <t>ASO ADM</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>ASO MUDANCA</t>
+    <t>sadad</t>
+  </si>
+  <si>
+    <t>sasad</t>
+  </si>
+  <si>
+    <t>saas</t>
   </si>
 </sst>
 </file>
@@ -393,7 +390,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,13 +407,17 @@
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
@@ -426,37 +427,29 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>